<commit_message>
update README file and data dictionary
</commit_message>
<xml_diff>
--- a/documentation/Data_Dictionary_with_Confounders.xlsx
+++ b/documentation/Data_Dictionary_with_Confounders.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RProjects\github\BRFSS\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B611FA-D776-49EB-92A7-776C9D95AF1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F46352-25A0-4C2C-96D0-3753D2249A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10500" yWindow="-13695" windowWidth="23340" windowHeight="11385" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="-14955" windowWidth="25980" windowHeight="11325" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Update histogram and boxplot
</commit_message>
<xml_diff>
--- a/documentation/Data_Dictionary_with_Confounders.xlsx
+++ b/documentation/Data_Dictionary_with_Confounders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RProjects\github\BRFSS\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F46352-25A0-4C2C-96D0-3753D2249A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3429009E-88E0-499B-BCB3-2F71C800B288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="-14955" windowWidth="25980" windowHeight="11325" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1212,7 +1212,7 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>

</xml_diff>